<commit_message>
Add new songs: WP-0331 -> WP-0345
</commit_message>
<xml_diff>
--- a/frontend/songlist/Jock's Karaoke De-duped.xlsx
+++ b/frontend/songlist/Jock's Karaoke De-duped.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6829" uniqueCount="5933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6874" uniqueCount="5972">
   <si>
     <t xml:space="preserve">4 Non Blondes </t>
   </si>
@@ -17819,6 +17819,123 @@
   </si>
   <si>
     <t>WP-0271</t>
+  </si>
+  <si>
+    <t>WP-0331</t>
+  </si>
+  <si>
+    <t>Simon &amp; Garfunkel</t>
+  </si>
+  <si>
+    <t>Cecilia</t>
+  </si>
+  <si>
+    <t>WP-0332</t>
+  </si>
+  <si>
+    <t>DeBarge</t>
+  </si>
+  <si>
+    <t>Rhythm of the Night</t>
+  </si>
+  <si>
+    <t>WP-0333</t>
+  </si>
+  <si>
+    <t>Solomon Burke</t>
+  </si>
+  <si>
+    <t>Cry to Me</t>
+  </si>
+  <si>
+    <t>WP-0334</t>
+  </si>
+  <si>
+    <t>Wouldn't it be Good</t>
+  </si>
+  <si>
+    <t>WP-0335</t>
+  </si>
+  <si>
+    <t>Something Blue</t>
+  </si>
+  <si>
+    <t>WP-0336</t>
+  </si>
+  <si>
+    <t>Lena Martell</t>
+  </si>
+  <si>
+    <t>One Day at a Time</t>
+  </si>
+  <si>
+    <t>WP-0337</t>
+  </si>
+  <si>
+    <t>Reef</t>
+  </si>
+  <si>
+    <t>Place Your Hands</t>
+  </si>
+  <si>
+    <t>WP-0338</t>
+  </si>
+  <si>
+    <t>Tom Odell</t>
+  </si>
+  <si>
+    <t>Another Love</t>
+  </si>
+  <si>
+    <t>WP-0339</t>
+  </si>
+  <si>
+    <t>O'Jays</t>
+  </si>
+  <si>
+    <t>Love Train</t>
+  </si>
+  <si>
+    <t>WP-0340</t>
+  </si>
+  <si>
+    <t>Secret Love</t>
+  </si>
+  <si>
+    <t>WP-0341</t>
+  </si>
+  <si>
+    <t>Queens of the Stone Age</t>
+  </si>
+  <si>
+    <t>No One Knows</t>
+  </si>
+  <si>
+    <t>WP-0342</t>
+  </si>
+  <si>
+    <t>Texas Hold 'Em</t>
+  </si>
+  <si>
+    <t>WP-0343</t>
+  </si>
+  <si>
+    <t>New Radicals</t>
+  </si>
+  <si>
+    <t>You Get What You Give</t>
+  </si>
+  <si>
+    <t>WP-0344</t>
+  </si>
+  <si>
+    <t>Chiquitita</t>
+  </si>
+  <si>
+    <t>WP-0345</t>
+  </si>
+  <si>
+    <t>I'm Every Woman</t>
   </si>
 </sst>
 </file>
@@ -18231,10 +18348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2277"/>
+  <dimension ref="A1:E2292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2259" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2225" sqref="D2225"/>
+    <sheetView tabSelected="1" topLeftCell="A2268" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2284" sqref="E2284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -43862,6 +43979,171 @@
       </c>
       <c r="C2277" s="10" t="s">
         <v>5889</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:3">
+      <c r="A2278" s="14" t="s">
+        <v>5933</v>
+      </c>
+      <c r="B2278" s="14" t="s">
+        <v>5934</v>
+      </c>
+      <c r="C2278" s="14" t="s">
+        <v>5935</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:3">
+      <c r="A2279" s="14" t="s">
+        <v>5936</v>
+      </c>
+      <c r="B2279" s="14" t="s">
+        <v>5937</v>
+      </c>
+      <c r="C2279" s="14" t="s">
+        <v>5938</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:3">
+      <c r="A2280" s="14" t="s">
+        <v>5939</v>
+      </c>
+      <c r="B2280" s="14" t="s">
+        <v>5940</v>
+      </c>
+      <c r="C2280" s="14" t="s">
+        <v>5941</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:3">
+      <c r="A2281" s="14" t="s">
+        <v>5942</v>
+      </c>
+      <c r="B2281" s="14" t="s">
+        <v>2298</v>
+      </c>
+      <c r="C2281" s="14" t="s">
+        <v>5943</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:3">
+      <c r="A2282" s="14" t="s">
+        <v>5944</v>
+      </c>
+      <c r="B2282" s="14" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C2282" s="14" t="s">
+        <v>5945</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:3">
+      <c r="A2283" s="14" t="s">
+        <v>5946</v>
+      </c>
+      <c r="B2283" s="14" t="s">
+        <v>5947</v>
+      </c>
+      <c r="C2283" s="14" t="s">
+        <v>5948</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:3">
+      <c r="A2284" s="14" t="s">
+        <v>5949</v>
+      </c>
+      <c r="B2284" s="14" t="s">
+        <v>5950</v>
+      </c>
+      <c r="C2284" s="14" t="s">
+        <v>5951</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:3">
+      <c r="A2285" s="14" t="s">
+        <v>5952</v>
+      </c>
+      <c r="B2285" s="14" t="s">
+        <v>5953</v>
+      </c>
+      <c r="C2285" s="14" t="s">
+        <v>5954</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:3">
+      <c r="A2286" s="14" t="s">
+        <v>5955</v>
+      </c>
+      <c r="B2286" s="14" t="s">
+        <v>5956</v>
+      </c>
+      <c r="C2286" s="14" t="s">
+        <v>5957</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:3">
+      <c r="A2287" s="14" t="s">
+        <v>5958</v>
+      </c>
+      <c r="B2287" s="14" t="s">
+        <v>2686</v>
+      </c>
+      <c r="C2287" s="14" t="s">
+        <v>5959</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:3">
+      <c r="A2288" s="14" t="s">
+        <v>5960</v>
+      </c>
+      <c r="B2288" s="14" t="s">
+        <v>5961</v>
+      </c>
+      <c r="C2288" s="14" t="s">
+        <v>5962</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:3">
+      <c r="A2289" s="14" t="s">
+        <v>5963</v>
+      </c>
+      <c r="B2289" s="14" t="s">
+        <v>833</v>
+      </c>
+      <c r="C2289" s="14" t="s">
+        <v>5964</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:3">
+      <c r="A2290" s="14" t="s">
+        <v>5965</v>
+      </c>
+      <c r="B2290" s="14" t="s">
+        <v>5966</v>
+      </c>
+      <c r="C2290" s="14" t="s">
+        <v>5967</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:3">
+      <c r="A2291" s="14" t="s">
+        <v>5968</v>
+      </c>
+      <c r="B2291" s="14" t="s">
+        <v>2794</v>
+      </c>
+      <c r="C2291" s="14" t="s">
+        <v>5969</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:3">
+      <c r="A2292" s="14" t="s">
+        <v>5970</v>
+      </c>
+      <c r="B2292" s="14" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2292" s="14" t="s">
+        <v>5971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>